<commit_message>
Adding German electricity mix for 2018
</commit_message>
<xml_diff>
--- a/data/inventory/lci-currentcars.xlsx
+++ b/data/inventory/lci-currentcars.xlsx
@@ -323,9 +323,6 @@
     <t>transport, passenger car, current, BEV, Van</t>
   </si>
   <si>
-    <t>market for electricity, low voltage</t>
-  </si>
-  <si>
     <t>DE</t>
   </si>
   <si>
@@ -333,6 +330,9 @@
   </si>
   <si>
     <t>Battery cell</t>
+  </si>
+  <si>
+    <t>market for electricity, low voltage, 2018</t>
   </si>
 </sst>
 </file>
@@ -400,13 +400,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Prozent" xfId="1" builtinId="5"/>
@@ -724,8 +725,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O810"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B8" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+    <sheetView tabSelected="1" topLeftCell="A636" workbookViewId="0">
+      <selection activeCell="A679" sqref="A679"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -742,7 +743,7 @@
         <v>65</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
@@ -8095,7 +8096,7 @@
     </row>
     <row r="460" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A460" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B460">
         <v>1.3500000000000001E-3</v>
@@ -8114,7 +8115,7 @@
       <c r="A461" t="s">
         <v>26</v>
       </c>
-      <c r="B461">
+      <c r="B461" s="6">
         <v>4.9999999999999998E-7</v>
       </c>
       <c r="C461" t="s">
@@ -8452,13 +8453,13 @@
     </row>
     <row r="478" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A478" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B478">
         <v>0.27226451522516532</v>
       </c>
       <c r="C478" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D478" t="s">
         <v>89</v>
@@ -8557,7 +8558,7 @@
     </row>
     <row r="490" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A490" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B490">
         <v>8.9999999999999998E-4</v>
@@ -8914,13 +8915,13 @@
     </row>
     <row r="508" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A508" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B508">
         <v>0.22677840134417709</v>
       </c>
       <c r="C508" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D508" t="s">
         <v>89</v>
@@ -9019,7 +9020,7 @@
     </row>
     <row r="520" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A520" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B520">
         <v>1.1999999999999999E-3</v>
@@ -9376,13 +9377,13 @@
     </row>
     <row r="538" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A538" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B538">
         <v>0.24992014246474201</v>
       </c>
       <c r="C538" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D538" t="s">
         <v>89</v>
@@ -9481,7 +9482,7 @@
     </row>
     <row r="550" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A550" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B550">
         <v>4.4999999999999999E-4</v>
@@ -9838,13 +9839,13 @@
     </row>
     <row r="568" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A568" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B568">
         <v>0.1850730728232271</v>
       </c>
       <c r="C568" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D568" t="s">
         <v>89</v>
@@ -9943,7 +9944,7 @@
     </row>
     <row r="580" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A580" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B580">
         <v>1.1999999999999999E-3</v>
@@ -10300,13 +10301,13 @@
     </row>
     <row r="598" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A598" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B598">
         <v>0.30496247112071961</v>
       </c>
       <c r="C598" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D598" t="s">
         <v>89</v>
@@ -10405,7 +10406,7 @@
     </row>
     <row r="610" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A610" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B610">
         <v>7.5000000000000002E-4</v>
@@ -10762,13 +10763,13 @@
     </row>
     <row r="628" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A628" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B628">
         <v>0.20321213645663391</v>
       </c>
       <c r="C628" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D628" t="s">
         <v>89</v>
@@ -10867,7 +10868,7 @@
     </row>
     <row r="640" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A640" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B640">
         <v>1.1999999999999999E-3</v>
@@ -11224,13 +11225,13 @@
     </row>
     <row r="658" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A658" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B658">
         <v>0.28773736333534028</v>
       </c>
       <c r="C658" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D658" t="s">
         <v>89</v>

</xml_diff>

<commit_message>
Adding LCA calculations for all cars
</commit_message>
<xml_diff>
--- a/data/inventory/lci-currentcars.xlsx
+++ b/data/inventory/lci-currentcars.xlsx
@@ -18,12 +18,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -339,8 +333,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000\ %"/>
+    <numFmt numFmtId="169" formatCode="0.0000000000"/>
+    <numFmt numFmtId="170" formatCode="0.00000000000"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -400,7 +396,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -408,6 +404,10 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Prozent" xfId="1" builtinId="5"/>
@@ -725,8 +725,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O810"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A636" workbookViewId="0">
-      <selection activeCell="A679" sqref="A679"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -736,6 +736,8 @@
     <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="68.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
@@ -1753,7 +1755,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>52</v>
       </c>
@@ -1773,7 +1775,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>54</v>
       </c>
@@ -1793,7 +1795,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="68" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>0</v>
       </c>
@@ -1801,7 +1803,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>2</v>
       </c>
@@ -1809,7 +1811,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>3</v>
       </c>
@@ -1817,7 +1819,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>5</v>
       </c>
@@ -1825,7 +1827,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>6</v>
       </c>
@@ -1833,12 +1835,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="73" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>9</v>
       </c>
@@ -1860,8 +1862,10 @@
       <c r="G74" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="L74" s="8"/>
+      <c r="M74" s="7"/>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>13</v>
       </c>
@@ -1877,8 +1881,10 @@
       <c r="F75" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="L75" s="8"/>
+      <c r="M75" s="7"/>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>17</v>
       </c>
@@ -1894,8 +1900,10 @@
       <c r="F76" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="L76" s="8"/>
+      <c r="M76" s="7"/>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>18</v>
       </c>
@@ -1911,8 +1919,10 @@
       <c r="F77" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="L77" s="8"/>
+      <c r="M77" s="7"/>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>19</v>
       </c>
@@ -1928,8 +1938,10 @@
       <c r="F78" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="L78" s="8"/>
+      <c r="M78" s="7"/>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>20</v>
       </c>
@@ -1945,8 +1957,10 @@
       <c r="F79" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="L79" s="8"/>
+      <c r="M79" s="7"/>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>21</v>
       </c>
@@ -1962,8 +1976,10 @@
       <c r="F80" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="L80" s="8"/>
+      <c r="M80" s="7"/>
+    </row>
+    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>22</v>
       </c>
@@ -1979,8 +1995,10 @@
       <c r="F81" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="L81" s="8"/>
+      <c r="M81" s="7"/>
+    </row>
+    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>23</v>
       </c>
@@ -1996,8 +2014,10 @@
       <c r="F82" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="L82" s="8"/>
+      <c r="M82" s="7"/>
+    </row>
+    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>24</v>
       </c>
@@ -2013,8 +2033,10 @@
       <c r="F83" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="L83" s="8"/>
+      <c r="M83" s="7"/>
+    </row>
+    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>25</v>
       </c>
@@ -2030,8 +2052,10 @@
       <c r="F84" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="L84" s="8"/>
+      <c r="M84" s="7"/>
+    </row>
+    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>26</v>
       </c>
@@ -2050,8 +2074,11 @@
       <c r="G85" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="L85" s="8"/>
+      <c r="M85" s="10"/>
+      <c r="N85" s="9"/>
+    </row>
+    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>29</v>
       </c>
@@ -2070,8 +2097,11 @@
       <c r="G86" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="L86" s="8"/>
+      <c r="M86" s="10"/>
+      <c r="N86" s="9"/>
+    </row>
+    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>31</v>
       </c>
@@ -2090,8 +2120,11 @@
       <c r="G87" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="L87" s="8"/>
+      <c r="M87" s="10"/>
+      <c r="N87" s="9"/>
+    </row>
+    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>33</v>
       </c>
@@ -2110,8 +2143,11 @@
       <c r="G88" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="L88" s="8"/>
+      <c r="M88" s="10"/>
+      <c r="N88" s="9"/>
+    </row>
+    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>36</v>
       </c>
@@ -2130,8 +2166,11 @@
       <c r="G89" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="L89" s="8"/>
+      <c r="M89" s="10"/>
+      <c r="N89" s="9"/>
+    </row>
+    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>38</v>
       </c>
@@ -2150,8 +2189,11 @@
       <c r="G90" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="L90" s="8"/>
+      <c r="M90" s="10"/>
+      <c r="N90" s="9"/>
+    </row>
+    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>38</v>
       </c>
@@ -2170,8 +2212,11 @@
       <c r="G91" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="L91" s="8"/>
+      <c r="M91" s="10"/>
+      <c r="N91" s="9"/>
+    </row>
+    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>40</v>
       </c>
@@ -2190,8 +2235,11 @@
       <c r="G92" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="L92" s="8"/>
+      <c r="M92" s="10"/>
+      <c r="N92" s="9"/>
+    </row>
+    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>42</v>
       </c>
@@ -2210,8 +2258,11 @@
       <c r="G93" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="L93" s="8"/>
+      <c r="M93" s="10"/>
+      <c r="N93" s="9"/>
+    </row>
+    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>44</v>
       </c>
@@ -2230,8 +2281,11 @@
       <c r="G94" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="L94" s="8"/>
+      <c r="M94" s="10"/>
+      <c r="N94" s="9"/>
+    </row>
+    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>48</v>
       </c>
@@ -2250,8 +2304,11 @@
       <c r="G95" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="L95" s="8"/>
+      <c r="M95" s="10"/>
+      <c r="N95" s="9"/>
+    </row>
+    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>50</v>
       </c>
@@ -2270,8 +2327,11 @@
       <c r="G96" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="L96" s="8"/>
+      <c r="M96" s="10"/>
+      <c r="N96" s="9"/>
+    </row>
+    <row r="97" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>52</v>
       </c>
@@ -2290,8 +2350,11 @@
       <c r="G97" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="L97" s="8"/>
+      <c r="M97" s="10"/>
+      <c r="N97" s="9"/>
+    </row>
+    <row r="98" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>54</v>
       </c>
@@ -2310,8 +2373,10 @@
       <c r="G98" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="100" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="M98" s="10"/>
+      <c r="N98" s="9"/>
+    </row>
+    <row r="100" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>0</v>
       </c>
@@ -2319,7 +2384,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>2</v>
       </c>
@@ -2327,7 +2392,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>3</v>
       </c>
@@ -2335,7 +2400,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>5</v>
       </c>
@@ -2343,7 +2408,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>6</v>
       </c>
@@ -2351,12 +2416,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="105" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>9</v>
       </c>
@@ -2379,7 +2444,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>13</v>
       </c>
@@ -2396,7 +2461,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>17</v>
       </c>
@@ -2413,7 +2478,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>18</v>
       </c>
@@ -2430,7 +2495,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>19</v>
       </c>
@@ -2447,7 +2512,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>20</v>
       </c>
@@ -2464,7 +2529,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>21</v>
       </c>

</xml_diff>

<commit_message>
Added input data to bev program
</commit_message>
<xml_diff>
--- a/data/inventory/lci-currentcars.xlsx
+++ b/data/inventory/lci-currentcars.xlsx
@@ -335,8 +335,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000\ %"/>
-    <numFmt numFmtId="169" formatCode="0.0000000000"/>
-    <numFmt numFmtId="170" formatCode="0.00000000000"/>
+    <numFmt numFmtId="165" formatCode="0.0000000000"/>
+    <numFmt numFmtId="166" formatCode="0.00000000000"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -404,9 +404,9 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
@@ -725,8 +725,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O810"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" topLeftCell="A622" workbookViewId="0">
+      <selection activeCell="F632" sqref="F632"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8520,8 +8520,8 @@
       <c r="A478" t="s">
         <v>100</v>
       </c>
-      <c r="B478">
-        <v>0.27226451522516532</v>
+      <c r="B478" s="2">
+        <v>0.28770167721950929</v>
       </c>
       <c r="C478" t="s">
         <v>97</v>
@@ -8982,8 +8982,8 @@
       <c r="A508" t="s">
         <v>100</v>
       </c>
-      <c r="B508">
-        <v>0.22677840134417709</v>
+      <c r="B508" s="2">
+        <v>0.16639850855058411</v>
       </c>
       <c r="C508" t="s">
         <v>97</v>
@@ -9444,8 +9444,8 @@
       <c r="A538" t="s">
         <v>100</v>
       </c>
-      <c r="B538">
-        <v>0.24992014246474201</v>
+      <c r="B538" s="2">
+        <v>0.21036558344273404</v>
       </c>
       <c r="C538" t="s">
         <v>97</v>
@@ -9906,8 +9906,8 @@
       <c r="A568" t="s">
         <v>100</v>
       </c>
-      <c r="B568">
-        <v>0.1850730728232271</v>
+      <c r="B568" s="2">
+        <v>0.16433797567998046</v>
       </c>
       <c r="C568" t="s">
         <v>97</v>
@@ -10368,8 +10368,8 @@
       <c r="A598" t="s">
         <v>100</v>
       </c>
-      <c r="B598">
-        <v>0.30496247112071961</v>
+      <c r="B598" s="2">
+        <v>0.30150037456114342</v>
       </c>
       <c r="C598" t="s">
         <v>97</v>
@@ -10830,8 +10830,8 @@
       <c r="A628" t="s">
         <v>100</v>
       </c>
-      <c r="B628">
-        <v>0.20321213645663391</v>
+      <c r="B628" s="2">
+        <v>0.16817553561518833</v>
       </c>
       <c r="C628" t="s">
         <v>97</v>
@@ -11292,8 +11292,8 @@
       <c r="A658" t="s">
         <v>100</v>
       </c>
-      <c r="B658">
-        <v>0.28773736333534028</v>
+      <c r="B658" s="2">
+        <v>0.21489603929826745</v>
       </c>
       <c r="C658" t="s">
         <v>97</v>
@@ -11338,5 +11338,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated HBEFA emission factors to 3.3
</commit_message>
<xml_diff>
--- a/data/inventory/lci-currentcars.xlsx
+++ b/data/inventory/lci-currentcars.xlsx
@@ -725,8 +725,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O810"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A622" workbookViewId="0">
-      <selection activeCell="F632" sqref="F632"/>
+    <sheetView tabSelected="1" topLeftCell="A658" workbookViewId="0">
+      <selection activeCell="B661" sqref="B661"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8521,7 +8521,7 @@
         <v>100</v>
       </c>
       <c r="B478" s="2">
-        <v>0.28770167721950929</v>
+        <v>0.27928701416120555</v>
       </c>
       <c r="C478" t="s">
         <v>97</v>
@@ -8983,7 +8983,7 @@
         <v>100</v>
       </c>
       <c r="B508" s="2">
-        <v>0.16639850855058411</v>
+        <v>0.15993345821425775</v>
       </c>
       <c r="C508" t="s">
         <v>97</v>
@@ -9445,7 +9445,7 @@
         <v>100</v>
       </c>
       <c r="B538" s="2">
-        <v>0.21036558344273404</v>
+        <v>0.20426776119815257</v>
       </c>
       <c r="C538" t="s">
         <v>97</v>
@@ -9907,7 +9907,7 @@
         <v>100</v>
       </c>
       <c r="B568" s="2">
-        <v>0.16433797567998046</v>
+        <v>0.15795271272604292</v>
       </c>
       <c r="C568" t="s">
         <v>97</v>
@@ -10369,7 +10369,7 @@
         <v>100</v>
       </c>
       <c r="B598" s="2">
-        <v>0.30150037456114342</v>
+        <v>0.29268022509102698</v>
       </c>
       <c r="C598" t="s">
         <v>97</v>
@@ -10831,7 +10831,7 @@
         <v>100</v>
       </c>
       <c r="B628" s="2">
-        <v>0.16817553561518833</v>
+        <v>0.16164122719548413</v>
       </c>
       <c r="C628" t="s">
         <v>97</v>
@@ -11293,7 +11293,7 @@
         <v>100</v>
       </c>
       <c r="B658" s="2">
-        <v>0.21489603929826745</v>
+        <v>0.20866542160597021</v>
       </c>
       <c r="C658" t="s">
         <v>97</v>

</xml_diff>